<commit_message>
Remodeled Crew Allocation data structures
</commit_message>
<xml_diff>
--- a/Crew_Allocation_Recap.xlsx
+++ b/Crew_Allocation_Recap.xlsx
@@ -22,6 +22,9 @@
     <t>Saturday, December 20, 2025</t>
   </si>
   <si>
+    <t>Last Name</t>
+  </si>
+  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -29,9 +32,6 @@
   </si>
   <si>
     <t>Equip</t>
-  </si>
-  <si>
-    <t>Last Name</t>
   </si>
   <si>
     <t>M</t>
@@ -455,17 +455,17 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Crew Allocation Excel Updated. Works for now
</commit_message>
<xml_diff>
--- a/Crew_Allocation_Recap.xlsx
+++ b/Crew_Allocation_Recap.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>TIMESHEET REVIEW / RECAP</t>
   </si>
   <si>
-    <t>Saturday, December 20, 2025</t>
+    <t>Saturday, January 31, 2026</t>
+  </si>
+  <si>
+    <t>Equip</t>
   </si>
   <si>
     <t>Last Name</t>
@@ -31,43 +34,118 @@
     <t>Class</t>
   </si>
   <si>
-    <t>Equip</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>12/15</t>
+    <t>01/26</t>
   </si>
   <si>
     <t>T</t>
   </si>
   <si>
-    <t>12/16</t>
+    <t>01/27</t>
   </si>
   <si>
     <t>W</t>
   </si>
   <si>
-    <t>12/17</t>
+    <t>01/28</t>
   </si>
   <si>
     <t>Th</t>
   </si>
   <si>
-    <t>12/18</t>
+    <t>01/29</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>12/19</t>
+    <t>01/30</t>
   </si>
   <si>
     <t>S</t>
   </si>
   <si>
-    <t>12/20</t>
+    <t>01/31</t>
+  </si>
+  <si>
+    <t>JOB 225010 Beador Rt 15 08-1K4004</t>
+  </si>
+  <si>
+    <t>Marin</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>LBSC1</t>
+  </si>
+  <si>
+    <t>225010</t>
+  </si>
+  <si>
+    <t>Palafox</t>
+  </si>
+  <si>
+    <t>Sergio</t>
+  </si>
+  <si>
+    <t>LBSD2</t>
+  </si>
+  <si>
+    <t>Espinoza</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>LBSC0</t>
+  </si>
+  <si>
+    <t>Richards</t>
+  </si>
+  <si>
+    <t>Doug</t>
+  </si>
+  <si>
+    <t>OPER1</t>
+  </si>
+  <si>
+    <t>Aguirre</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Valdivia</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>LISC4</t>
+  </si>
+  <si>
+    <t>Ortiz</t>
+  </si>
+  <si>
+    <t>Gilberto</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>LISC6</t>
+  </si>
+  <si>
+    <t>Avila</t>
+  </si>
+  <si>
+    <t>Agustin</t>
+  </si>
+  <si>
+    <t>LBSC7</t>
   </si>
 </sst>
 </file>
@@ -456,16 +534,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -484,6 +562,186 @@
       </c>
       <c r="K5" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ReportService and domain structures for daily reports functionality
</commit_message>
<xml_diff>
--- a/Crew_Allocation_Recap.xlsx
+++ b/Crew_Allocation_Recap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>TIMESHEET REVIEW / RECAP</t>
   </si>
@@ -22,18 +22,18 @@
     <t>Saturday, January 31, 2026</t>
   </si>
   <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
     <t>Equip</t>
   </si>
   <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -73,79 +73,103 @@
     <t>JOB 225010 Beador Rt 15 08-1K4004</t>
   </si>
   <si>
+    <t>Aguirre</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>LBSC1</t>
+  </si>
+  <si>
+    <t>225010</t>
+  </si>
+  <si>
+    <t>Richards</t>
+  </si>
+  <si>
+    <t>Doug</t>
+  </si>
+  <si>
+    <t>OPER1</t>
+  </si>
+  <si>
+    <t>Palafox</t>
+  </si>
+  <si>
+    <t>Sergio</t>
+  </si>
+  <si>
+    <t>LBSD2</t>
+  </si>
+  <si>
+    <t>Avila</t>
+  </si>
+  <si>
+    <t>Agustin</t>
+  </si>
+  <si>
+    <t>LBSC7</t>
+  </si>
+  <si>
+    <t>225010 / 225010</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>LISC6</t>
+  </si>
+  <si>
+    <t>Calixto</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>P-AP5</t>
+  </si>
+  <si>
+    <t>Lomeli</t>
+  </si>
+  <si>
+    <t>Trinidad</t>
+  </si>
+  <si>
+    <t>P-FF</t>
+  </si>
+  <si>
+    <t>Valdivia</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>LISC4</t>
+  </si>
+  <si>
+    <t>Ortiz</t>
+  </si>
+  <si>
+    <t>Gilberto</t>
+  </si>
+  <si>
+    <t>LBSC0</t>
+  </si>
+  <si>
     <t>Marin</t>
   </si>
   <si>
-    <t>Jesus</t>
-  </si>
-  <si>
-    <t>LBSC1</t>
-  </si>
-  <si>
-    <t>225010</t>
-  </si>
-  <si>
-    <t>Palafox</t>
-  </si>
-  <si>
-    <t>Sergio</t>
-  </si>
-  <si>
-    <t>LBSD2</t>
-  </si>
-  <si>
-    <t>Espinoza</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>LBSC0</t>
-  </si>
-  <si>
-    <t>Richards</t>
-  </si>
-  <si>
-    <t>Doug</t>
-  </si>
-  <si>
-    <t>OPER1</t>
-  </si>
-  <si>
-    <t>Aguirre</t>
-  </si>
-  <si>
-    <t>Santiago</t>
-  </si>
-  <si>
-    <t>Valdivia</t>
-  </si>
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>LISC4</t>
-  </si>
-  <si>
-    <t>Ortiz</t>
-  </si>
-  <si>
-    <t>Gilberto</t>
-  </si>
-  <si>
-    <t>Garcia</t>
-  </si>
-  <si>
-    <t>LISC6</t>
-  </si>
-  <si>
-    <t>Avila</t>
-  </si>
-  <si>
-    <t>Agustin</t>
-  </si>
-  <si>
-    <t>LBSC7</t>
+    <t>Causey</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>OPEA4</t>
   </si>
 </sst>
 </file>
@@ -534,16 +558,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -589,6 +613,12 @@
       <c r="H8" t="s">
         <v>22</v>
       </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -600,13 +630,16 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
       <c r="G9" t="s">
         <v>22</v>
       </c>
       <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -620,10 +653,19 @@
       <c r="C10" t="s">
         <v>28</v>
       </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
       <c r="G10" t="s">
         <v>22</v>
       </c>
       <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -637,22 +679,31 @@
       <c r="C11" t="s">
         <v>31</v>
       </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
       <c r="G11" t="s">
         <v>22</v>
       </c>
       <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
@@ -661,58 +712,58 @@
         <v>22</v>
       </c>
       <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
@@ -721,18 +772,24 @@
         <v>22</v>
       </c>
       <c r="H15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
@@ -741,6 +798,52 @@
         <v>22</v>
       </c>
       <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>